<commit_message>
31 de Marzo 2023
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #01   ENERO 2023/REMISIONES  CENTRAL  ENERO 2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #01   ENERO 2023/REMISIONES  CENTRAL  ENERO 2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19830" windowHeight="11670" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19830" windowHeight="11670" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O      2 0 2 3    " sheetId="1" r:id="rId1"/>
@@ -7790,7 +7790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+    <sheetView topLeftCell="A184" workbookViewId="0">
       <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
@@ -13971,654 +13971,654 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H29"/>
+  <dimension ref="B3:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5">
+      <c r="C5" s="5">
         <v>11249</v>
       </c>
-      <c r="C5" s="12">
+      <c r="D5" s="12">
         <v>9310.4</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="12">
+      <c r="F5" s="12">
         <v>9310.4</v>
       </c>
-      <c r="F5" s="12">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" s="7" t="s">
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9">
+      <c r="C6" s="9">
         <v>11253</v>
       </c>
-      <c r="C6" s="13">
+      <c r="D6" s="13">
         <v>6726</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="13">
+      <c r="F6" s="13">
         <v>6726</v>
       </c>
-      <c r="F6" s="13">
-        <v>0</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="G6" s="13">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="9">
+      <c r="C7" s="9">
         <v>11256</v>
       </c>
-      <c r="C7" s="13">
+      <c r="D7" s="13">
         <v>600</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="13">
+      <c r="F7" s="13">
         <v>600</v>
       </c>
-      <c r="F7" s="13">
-        <v>0</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="G7" s="13">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5">
+      <c r="C8" s="5">
         <v>11260</v>
       </c>
-      <c r="C8" s="12">
+      <c r="D8" s="12">
         <v>9360</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="12">
+      <c r="F8" s="12">
         <v>9360</v>
       </c>
-      <c r="F8" s="12">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5">
+      <c r="C9" s="5">
         <v>11264</v>
       </c>
-      <c r="C9" s="12">
+      <c r="D9" s="12">
         <v>360</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="12">
+      <c r="F9" s="12">
         <v>360</v>
       </c>
-      <c r="F9" s="12">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="9">
+      <c r="C10" s="9">
         <v>11269</v>
       </c>
-      <c r="C10" s="13">
+      <c r="D10" s="13">
         <v>360</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="13">
+      <c r="F10" s="13">
         <v>360</v>
       </c>
-      <c r="F10" s="13">
-        <v>0</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="G10" s="13">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="9">
+      <c r="C11" s="9">
         <v>11277</v>
       </c>
-      <c r="C11" s="13">
+      <c r="D11" s="13">
         <v>9486.4</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="13">
+      <c r="F11" s="13">
         <v>9486.4</v>
       </c>
-      <c r="F11" s="13">
-        <v>0</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="G11" s="13">
+        <v>0</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="9">
+      <c r="C12" s="9">
         <v>11291</v>
       </c>
-      <c r="C12" s="13">
+      <c r="D12" s="13">
         <v>3878.4</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="13">
+      <c r="F12" s="13">
         <v>3878.4</v>
       </c>
-      <c r="F12" s="13">
-        <v>0</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="9">
+      <c r="C13" s="9">
         <v>11302</v>
       </c>
-      <c r="C13" s="13">
+      <c r="D13" s="13">
         <v>480</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="13">
+      <c r="F13" s="13">
         <v>480</v>
       </c>
-      <c r="F13" s="13">
-        <v>0</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="G13" s="13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="9">
+      <c r="C14" s="9">
         <v>11309</v>
       </c>
-      <c r="C14" s="13">
+      <c r="D14" s="13">
         <v>9404</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="13">
+      <c r="F14" s="13">
         <v>9404</v>
       </c>
-      <c r="F14" s="13">
-        <v>0</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="9">
+      <c r="C15" s="9">
         <v>11329</v>
       </c>
-      <c r="C15" s="13">
+      <c r="D15" s="13">
         <v>10195.200000000001</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="13">
+      <c r="F15" s="13">
         <v>10195.200000000001</v>
       </c>
-      <c r="F15" s="13">
-        <v>0</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="G15" s="13">
+        <v>0</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="9">
+      <c r="C16" s="9">
         <v>11341</v>
       </c>
-      <c r="C16" s="13">
+      <c r="D16" s="13">
         <v>600</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="13">
+      <c r="F16" s="13">
         <v>600</v>
       </c>
-      <c r="F16" s="13">
-        <v>0</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="G16" s="13">
+        <v>0</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="5">
+      <c r="C17" s="5">
         <v>11342</v>
       </c>
-      <c r="C17" s="12">
+      <c r="D17" s="12">
         <v>360</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="12">
+      <c r="F17" s="12">
         <v>360</v>
       </c>
-      <c r="F17" s="12">
-        <v>0</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="G17" s="12">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="9">
+      <c r="C18" s="9">
         <v>11349</v>
       </c>
-      <c r="C18" s="13">
+      <c r="D18" s="13">
         <v>480</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="13">
+      <c r="F18" s="13">
         <v>480</v>
       </c>
-      <c r="F18" s="13">
-        <v>0</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="G18" s="13">
+        <v>0</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="5">
+      <c r="C19" s="5">
         <v>11362</v>
       </c>
-      <c r="C19" s="12">
+      <c r="D19" s="12">
         <v>9720.7999999999993</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="12">
+      <c r="F19" s="12">
         <v>9720.7999999999993</v>
       </c>
-      <c r="F19" s="12">
-        <v>0</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="G19" s="12">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="5">
+      <c r="C20" s="5">
         <v>11376</v>
       </c>
-      <c r="C20" s="12">
+      <c r="D20" s="12">
         <v>480</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="12">
+      <c r="F20" s="12">
         <v>480</v>
       </c>
-      <c r="F20" s="12">
-        <v>0</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="G20" s="12">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="9">
+      <c r="C21" s="9">
         <v>11390</v>
       </c>
-      <c r="C21" s="13">
+      <c r="D21" s="13">
         <v>480</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="13">
-        <v>0</v>
-      </c>
+      <c r="E21" s="10"/>
       <c r="F21" s="13">
+        <v>0</v>
+      </c>
+      <c r="G21" s="13">
         <v>480</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="H21" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="H21" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="I21" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="9">
+      <c r="C22" s="9">
         <v>11395</v>
       </c>
-      <c r="C22" s="13">
+      <c r="D22" s="13">
         <v>9412.7999999999993</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="13">
-        <v>0</v>
-      </c>
+      <c r="E22" s="10"/>
       <c r="F22" s="13">
+        <v>0</v>
+      </c>
+      <c r="G22" s="13">
         <v>9412.7999999999993</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="H22" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="I22" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="5">
+      <c r="C23" s="5">
         <v>11397</v>
       </c>
-      <c r="C23" s="12">
+      <c r="D23" s="12">
         <v>360</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="12">
-        <v>0</v>
-      </c>
+      <c r="E23" s="6"/>
       <c r="F23" s="12">
+        <v>0</v>
+      </c>
+      <c r="G23" s="12">
         <v>360</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="H23" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H23" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="I23" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="9">
+      <c r="C24" s="9">
         <v>11407</v>
       </c>
-      <c r="C24" s="13">
+      <c r="D24" s="13">
         <v>480</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="13">
-        <v>0</v>
-      </c>
+      <c r="E24" s="10"/>
       <c r="F24" s="13">
+        <v>0</v>
+      </c>
+      <c r="G24" s="13">
         <v>480</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="H24" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="H24" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="I24" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="5">
+      <c r="C25" s="5">
         <v>11432</v>
       </c>
-      <c r="C25" s="12">
+      <c r="D25" s="12">
         <v>360</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="12">
-        <v>0</v>
-      </c>
+      <c r="E25" s="6"/>
       <c r="F25" s="12">
+        <v>0</v>
+      </c>
+      <c r="G25" s="12">
         <v>360</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="H25" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H25" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="I25" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="5">
+      <c r="C26" s="5">
         <v>11434</v>
       </c>
-      <c r="C26" s="12">
+      <c r="D26" s="12">
         <v>4240</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="12">
-        <v>0</v>
-      </c>
+      <c r="E26" s="6"/>
       <c r="F26" s="12">
+        <v>0</v>
+      </c>
+      <c r="G26" s="12">
         <v>4240</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="H26" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H26" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="I26" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="9">
+      <c r="C27" s="9">
         <v>11437</v>
       </c>
-      <c r="C27" s="13">
+      <c r="D27" s="13">
         <v>480</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="13">
-        <v>0</v>
-      </c>
+      <c r="E27" s="10"/>
       <c r="F27" s="13">
+        <v>0</v>
+      </c>
+      <c r="G27" s="13">
         <v>480</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="H27" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="H27" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="I27" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="5">
+      <c r="C28" s="5">
         <v>11442</v>
       </c>
-      <c r="C28" s="12">
+      <c r="D28" s="12">
         <v>9707.2000000000007</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="12">
-        <v>0</v>
-      </c>
+      <c r="E28" s="6"/>
       <c r="F28" s="12">
+        <v>0</v>
+      </c>
+      <c r="G28" s="12">
         <v>9707.2000000000007</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="H28" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H28" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="I28" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="9">
+      <c r="C29" s="9">
         <v>11455</v>
       </c>
-      <c r="C29" s="13">
+      <c r="D29" s="13">
         <v>480</v>
       </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="13">
-        <v>0</v>
-      </c>
+      <c r="E29" s="10"/>
       <c r="F29" s="13">
+        <v>0</v>
+      </c>
+      <c r="G29" s="13">
         <v>480</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="H29" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="I29" s="11" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>